<commit_message>
update/bugfix EV charging power time series
</commit_message>
<xml_diff>
--- a/ev_charging/ev_profile_generation/Statistics.xlsx
+++ b/ev_charging/ev_profile_generation/Statistics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\heat-pumps-grid-interaction\ev\ev_profile_generation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\EBC_ACS0025_EONgGmbH_HybridWP_\Data\Work Data Sebastian\heat-pumps-grid-interaction\ev_charging\ev_profile_generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1830" windowWidth="21600" windowHeight="11295" activeTab="4"/>
+    <workbookView xWindow="2445" yWindow="1830" windowWidth="21600" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="TimeID" sheetId="1" r:id="rId1"/>
@@ -492,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -992,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>